<commit_message>
polymer class test study
</commit_message>
<xml_diff>
--- a/3a.1.PlasticsAndCompositesEngineering/8_FinalTerm/CauseEffectCompilation.xlsx
+++ b/3a.1.PlasticsAndCompositesEngineering/8_FinalTerm/CauseEffectCompilation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_d08\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tecmx-my.sharepoint.com/personal/a01212611_itesm_mx/Documents/Documents/MNT_ITESM_courses/3a.1.PlasticsAndCompositesEngineering/8_FinalTerm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="268" documentId="8_{3543B509-ADE6-441A-AAF1-2D4CA3E76EE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AFF53FBC-A84C-4CCD-A16F-9A4482FD293C}"/>
+  <xr:revisionPtr revIDLastSave="292" documentId="8_{3543B509-ADE6-441A-AAF1-2D4CA3E76EE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{60DA6D6C-E8C1-4BBA-9E39-BDDE96C96FFE}"/>
   <bookViews>
-    <workbookView xWindow="13980" yWindow="3225" windowWidth="20685" windowHeight="11835" xr2:uid="{DB3E3740-E930-45AD-AE3C-4F4684730B06}"/>
+    <workbookView xWindow="8460" yWindow="1155" windowWidth="20685" windowHeight="11835" xr2:uid="{DB3E3740-E930-45AD-AE3C-4F4684730B06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="74">
   <si>
     <t>Plastics and Composites Engineering</t>
   </si>
@@ -114,15 +114,9 @@
     <t>viscosity's shear thinning behavior</t>
   </si>
   <si>
-    <t>branch density</t>
-  </si>
-  <si>
     <t>viscosity</t>
   </si>
   <si>
-    <t>shouldn't viscosity increase?</t>
-  </si>
-  <si>
     <t>entanglement</t>
   </si>
   <si>
@@ -247,6 +241,24 @@
   </si>
   <si>
     <t>relaxation modulus</t>
+  </si>
+  <si>
+    <t>crystall content</t>
+  </si>
+  <si>
+    <t>difficulty to shear</t>
+  </si>
+  <si>
+    <t>deformation time</t>
+  </si>
+  <si>
+    <t>molecular weight</t>
+  </si>
+  <si>
+    <t>humidity</t>
+  </si>
+  <si>
+    <t>viscoelasticity</t>
   </si>
 </sst>
 </file>
@@ -796,8 +808,8 @@
   <dimension ref="A1:G104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,7 +963,7 @@
         <v>13</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>18</v>
@@ -1088,16 +1100,13 @@
         <v>9</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1111,13 +1120,13 @@
         <v>9</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1131,13 +1140,13 @@
         <v>9</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1151,13 +1160,13 @@
         <v>12</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1171,13 +1180,13 @@
         <v>9</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1188,16 +1197,16 @@
         <v>8</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1208,16 +1217,16 @@
         <v>8</v>
       </c>
       <c r="C21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>35</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1237,10 +1246,10 @@
         <v>9</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1248,19 +1257,19 @@
         <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1268,19 +1277,19 @@
         <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1288,19 +1297,19 @@
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1308,19 +1317,19 @@
         <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1328,19 +1337,19 @@
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1348,19 +1357,19 @@
         <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1368,19 +1377,19 @@
         <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1388,19 +1397,19 @@
         <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1408,19 +1417,19 @@
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1428,19 +1437,19 @@
         <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1448,19 +1457,19 @@
         <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1468,19 +1477,19 @@
         <v>30</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1488,19 +1497,19 @@
         <v>31</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1508,22 +1517,22 @@
         <v>32</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1537,13 +1546,13 @@
         <v>9</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1557,13 +1566,13 @@
         <v>9</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1577,28 +1586,73 @@
         <v>9</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>36</v>
       </c>
+      <c r="B40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>37</v>
       </c>
+      <c r="B41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>38</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1983,15 +2037,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000FDFDB931CEC1A4D9173FDD6F623054F" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f31d27728cc3f5d8bc0ebea293483bad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e2309a97-5dbe-4782-af0a-c6fa888d645b" xmlns:ns4="faf185f4-fa7c-4454-b7fc-1060ac3b9dc2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4875a9bdfac96ec451fdfd88f66794e" ns3:_="" ns4:_="">
     <xsd:import namespace="e2309a97-5dbe-4782-af0a-c6fa888d645b"/>
@@ -2214,6 +2259,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{570E4CEA-8FBA-4B91-A78D-89E239A293F5}">
   <ds:schemaRefs>
@@ -2224,14 +2278,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C32259CD-D2A1-4BA7-BCD2-3D5C2FFAF372}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{821F291D-B562-4450-BE78-56AFB86F2C75}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2248,4 +2294,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C32259CD-D2A1-4BA7-BCD2-3D5C2FFAF372}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>